<commit_message>
changed events title heading
</commit_message>
<xml_diff>
--- a/public/main_page/events_data.xlsx
+++ b/public/main_page/events_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15413\Desktop\Alex\Clean 3\Projects\shpe_website\my_shpe_website\public\main_page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB8C976-7A10-48D2-9A34-81C5FD222516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC30A503-CBF4-4E9D-B115-895883BAA30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,9 +112,6 @@
     <t>Study &amp; Sweets: A Valentine's Study Session</t>
   </si>
   <si>
-    <t>Upcoming Events</t>
-  </si>
-  <si>
     <t>Join us for our next study session with a fun twist—an elementary school-style Valentine’s exchange! Bring your own Valentines to swap, and we’ll have supplies to make cards so no one is left out.</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t>STUDY SESSIONS</t>
   </si>
   <si>
-    <t>Thursdays!</t>
-  </si>
-  <si>
     <t>Lock in &amp; study with us!</t>
   </si>
   <si>
@@ -137,6 +131,12 @@
   </si>
   <si>
     <t>Every Thursday, 7-10PM. EB315</t>
+  </si>
+  <si>
+    <t>Upcoming Events!</t>
+  </si>
+  <si>
+    <t>Every Thursday!</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -446,36 +446,36 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>
       </c>
       <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="D3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>